<commit_message>
Starting Extracting data from pitchers
</commit_message>
<xml_diff>
--- a/Scrum/Proyect/Agile-product-backlog-template.xlsx
+++ b/Scrum/Proyect/Agile-product-backlog-template.xlsx
@@ -1,151 +1,137 @@
 
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisma\Documents\Visual Studio 2015\Projects\WindowsFormsApplication3\Scrum\Templates\2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="12000" yWindow="0" windowWidth="29055" windowHeight="19635" tabRatio="500"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-  </sheets>
-  <definedNames>
-    <definedName name="Priority">Sheet2!$B$6:$B$8</definedName>
-    <definedName name="Status">Sheet2!$C$6:$C$8</definedName>
-    <definedName name="YesNo">Sheet2!$A$6:$A$7</definedName>
-  </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
-</workbook>
+<file path=docProps\app.xml><?xml version="1.0" encoding="utf-8"?>
+<Properties xmlns="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <Application>Microsoft Excel</Application>
+  <DocSecurity>0</DocSecurity>
+  <ScaleCrop>false</ScaleCrop>
+  <HeadingPairs>
+    <vt:vector size="4" baseType="variant">
+      <vt:variant>
+        <vt:lpstr>Worksheets</vt:lpstr>
+      </vt:variant>
+      <vt:variant>
+        <vt:i4>2</vt:i4>
+      </vt:variant>
+      <vt:variant>
+        <vt:lpstr>Named Ranges</vt:lpstr>
+      </vt:variant>
+      <vt:variant>
+        <vt:i4>3</vt:i4>
+      </vt:variant>
+    </vt:vector>
+  </HeadingPairs>
+  <TitlesOfParts>
+    <vt:vector size="5" baseType="lpstr">
+      <vt:lpstr>Sheet1</vt:lpstr>
+      <vt:lpstr>Sheet2</vt:lpstr>
+      <vt:lpstr>Priority</vt:lpstr>
+      <vt:lpstr>Status</vt:lpstr>
+      <vt:lpstr>YesNo</vt:lpstr>
+    </vt:vector>
+  </TitlesOfParts>
+  <Company/>
+  <LinksUpToDate>false</LinksUpToDate>
+  <SharedDoc>false</SharedDoc>
+  <HyperlinksChanged>false</HyperlinksChanged>
+  <AppVersion>15.0300</AppVersion>
+</Properties>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="37">
-  <si>
-    <t>Task Name</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Story Points</t>
-  </si>
-  <si>
-    <t>Assigned to Sprint</t>
-  </si>
-  <si>
-    <t>Sprint Ready</t>
-  </si>
-  <si>
-    <t>Story</t>
-  </si>
-  <si>
-    <t>Sprint 1</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>Task 12</t>
-  </si>
-  <si>
-    <t>Sprint 5</t>
-  </si>
-  <si>
-    <t>Task 13</t>
-  </si>
-  <si>
-    <t>Task 14</t>
-  </si>
-  <si>
-    <t>Task 15</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Not Started</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This sheet is to enable the drop-down lists </t>
-  </si>
-  <si>
-    <t>Agile Product Backlog</t>
-  </si>
-  <si>
-    <t>Create a Product Backlog in Smartsheet</t>
-  </si>
-  <si>
-    <t>Extract MLB Stats</t>
-  </si>
-  <si>
-    <t>Extract MLB Schedule</t>
-  </si>
-  <si>
-    <t>Extract MLB Series</t>
-  </si>
-  <si>
-    <t>Align MLB Series per day</t>
-  </si>
-  <si>
-    <t>Create class/DB model with data</t>
-  </si>
-  <si>
-    <t>Create MLB Game Class</t>
-  </si>
-  <si>
-    <t>Extract data from team</t>
-  </si>
-  <si>
-    <t>Fill data periodically</t>
-  </si>
-  <si>
-    <t>Creting of sheets depending of quantities and dates</t>
-  </si>
-  <si>
-    <t>Order schedule</t>
-  </si>
-  <si>
-    <t>Create MLB Serie class</t>
-  </si>
-  <si>
-    <t>http://www.covers.com/pageLoader/pageLoader.aspx?page=/data/mlb/matchups/g4_summary_12.html</t>
-  </si>
-</sst>
+<file path=docProps\core.xml><?xml version="1.0" encoding="utf-8"?>
+<cp:coreProperties xmlns:cp="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:dcmitype="http://purl.org/dc/dcmitype/" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <dc:creator>Emily Esposito</dc:creator>
+  <cp:lastModifiedBy>Luis Matamoros Araya</cp:lastModifiedBy>
+  <dcterms:created xsi:type="dcterms:W3CDTF">2016-02-17T17:32:45Z</dcterms:created>
+  <dcterms:modified xsi:type="dcterms:W3CDTF">2017-08-18T20:56:08Z</dcterms:modified>
+</cp:coreProperties>
 </file>
 
-<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl\drawings\drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>103216</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1473200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6997700" y="293716"/>
+          <a:ext cx="2425700" cy="544483"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>84797</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>14345</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9279597"/>
+          <a:ext cx="14351000" cy="4311048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl\sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+</file>
+
+<file path=xl\styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -310,88 +296,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>103216</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1473200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>165099</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6997700" y="293716"/>
-          <a:ext cx="2425700" cy="544483"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>84797</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>14345</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="9279597"/>
-          <a:ext cx="14351000" cy="4311048"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl\theme\theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -711,7 +616,37 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl\workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisma\Documents\Visual Studio 2015\Projects\WindowsFormsApplication3\Scrum\Templates\2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="12000" yWindow="0" windowWidth="29055" windowHeight="19635" tabRatio="500"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+  </sheets>
+  <definedNames>
+    <definedName name="Priority">Sheet2!$B$6:$B$8</definedName>
+    <definedName name="Status">Sheet2!$C$6:$C$8</definedName>
+    <definedName name="YesNo">Sheet2!$A$6:$A$7</definedName>
+  </definedNames>
+  <calcPr calcId="152511" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=xl\worksheets\sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC72"/>
   <sheetViews>
@@ -792,8 +727,10 @@
       <c r="AC2" s="5"/>
     </row>
     <row r="3" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>23</v>
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Agile Product Backlog</t>
+        </is>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -887,26 +824,40 @@
       <c r="AC5" s="5"/>
     </row>
     <row r="6" spans="1:29" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>4</v>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Task Name</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>Story</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>Sprint Ready</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>Priority</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>Story Points</t>
+        </is>
+      </c>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>Assigned to Sprint</t>
+        </is>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -932,27 +883,38 @@
       <c r="AC6" s="5"/>
     </row>
     <row r="7" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>20</v>
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Sprint 1</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
       </c>
       <c r="F7" s="3">
         <f>SUM(F8:F10)</f>
-        <v>24</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>15</v>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -978,26 +940,38 @@
       <c r="AC7" s="5"/>
     </row>
     <row r="8" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>19</v>
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>Extract MLB Stats</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
       </c>
       <c r="F8" s="2">
         <v>8</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>14</v>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -1023,26 +997,38 @@
       <c r="AC8" s="5"/>
     </row>
     <row r="9" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>19</v>
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>Extract MLB Schedule</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
       </c>
       <c r="F9" s="2">
         <v>16</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>14</v>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -1068,26 +1054,38 @@
       <c r="AC9" s="5"/>
     </row>
     <row r="10" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>Extract MLB Series</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
       </c>
       <c r="F10" s="2">
         <v>0</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>14</v>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -1116,8 +1114,10 @@
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>36</v>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>http://www.covers.com/pageLoader/pageLoader.aspx?page=/data/mlb/matchups/g4_summary_12.html</t>
+        </is>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1146,26 +1146,38 @@
       <c r="AC11" s="5"/>
     </row>
     <row r="12" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>19</v>
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t>Align MLB Series per day</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
       </c>
       <c r="F12" s="2">
         <v>32</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>14</v>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -1191,26 +1203,38 @@
       <c r="AC12" s="5"/>
     </row>
     <row r="13" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>19</v>
+      <c r="A13" s="8" t="inlineStr">
+        <is>
+          <t>Create class/DB model with data</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
       </c>
       <c r="F13" s="2">
         <v>48</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>14</v>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -1236,26 +1260,38 @@
       <c r="AC13" s="5"/>
     </row>
     <row r="14" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>21</v>
+      <c r="A14" s="8" t="inlineStr">
+        <is>
+          <t>Create MLB Game Class</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
       </c>
       <c r="F14" s="2">
         <v>16</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>15</v>
+      <c r="G14" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -1312,26 +1348,38 @@
       <c r="AC15" s="5"/>
     </row>
     <row r="16" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>20</v>
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>Create MLB Serie class</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
       </c>
       <c r="F16" s="2">
         <v>8</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>15</v>
+      <c r="G16" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
@@ -1357,26 +1405,38 @@
       <c r="AC16" s="5"/>
     </row>
     <row r="17" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>20</v>
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Extract data from team</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
       </c>
       <c r="F17" s="2">
         <v>8</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>15</v>
+      <c r="G17" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1402,26 +1462,38 @@
       <c r="AC17" s="5"/>
     </row>
     <row r="18" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>20</v>
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Fill data periodically</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
       </c>
       <c r="F18" s="2">
         <v>16</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>15</v>
+      <c r="G18" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
@@ -1447,27 +1519,38 @@
       <c r="AC18" s="5"/>
     </row>
     <row r="19" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>20</v>
+      <c r="A19" s="3" t="inlineStr">
+        <is>
+          <t>Sprint 4</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E19" s="3" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
       </c>
       <c r="F19" s="3">
         <f>SUM(F20:F22)</f>
-        <v>64</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>14</v>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1493,26 +1576,38 @@
       <c r="AC19" s="5"/>
     </row>
     <row r="20" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>20</v>
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>Creting of sheets depending of quantities and dates</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
       </c>
       <c r="F20" s="2">
         <v>32</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>15</v>
+      <c r="G20" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
@@ -1538,26 +1633,38 @@
       <c r="AC20" s="5"/>
     </row>
     <row r="21" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>19</v>
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>Order schedule</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
       </c>
       <c r="F21" s="2">
         <v>32</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>14</v>
+      <c r="G21" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -1583,26 +1690,38 @@
       <c r="AC21" s="5"/>
     </row>
     <row r="22" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>19</v>
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Task 12</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
       </c>
       <c r="F22" s="2">
         <v>0</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>14</v>
+      <c r="G22" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
@@ -1628,27 +1747,38 @@
       <c r="AC22" s="5"/>
     </row>
     <row r="23" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>21</v>
+      <c r="A23" s="3" t="inlineStr">
+        <is>
+          <t>Sprint 5</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E23" s="3" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
       </c>
       <c r="F23" s="3">
         <f>SUM(F24:F26)</f>
-        <v>64</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>15</v>
+      </c>
+      <c r="G23" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -1674,26 +1804,38 @@
       <c r="AC23" s="5"/>
     </row>
     <row r="24" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>21</v>
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>Task 13</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
       </c>
       <c r="F24" s="2">
         <v>48</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>15</v>
+      <c r="G24" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -1719,26 +1861,38 @@
       <c r="AC24" s="5"/>
     </row>
     <row r="25" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>21</v>
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>Task 14</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
       </c>
       <c r="F25" s="2">
         <v>8</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>15</v>
+      <c r="G25" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -1764,26 +1918,38 @@
       <c r="AC25" s="5"/>
     </row>
     <row r="26" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>21</v>
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>Task 15</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
       </c>
       <c r="F26" s="2">
         <v>8</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>15</v>
+      <c r="G26" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -1871,8 +2037,10 @@
       <c r="AC28" s="5"/>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>24</v>
+      <c r="A29" s="9" t="inlineStr">
+        <is>
+          <t>Create a Product Backlog in Smartsheet</t>
+        </is>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -3335,7 +3503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl\worksheets\sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C8"/>
   <sheetViews>
@@ -3346,38 +3514,56 @@
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>22</v>
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This sheet is to enable the drop-down lists </t>
+        </is>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Not Started</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>